<commit_message>
rcs rus teg added
</commit_message>
<xml_diff>
--- a/Textbooks, projects/Organization and management of production activities/latyshov/cgt_latyshov.xlsx
+++ b/Textbooks, projects/Organization and management of production activities/latyshov/cgt_latyshov.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74FB1D2-FAA2-4E4C-9B2B-E229A15A82EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4688F77-2A1F-47A2-B399-B1F6B779B52F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a_r=0.5" sheetId="1" r:id="rId1"/>
@@ -28504,8 +28504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4092CB23-280F-4689-BAC4-4FA97EF9B777}">
   <dimension ref="A3:L171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57569,8 +57569,8 @@
   <sheetPr codeName="Лист8"/>
   <dimension ref="A1:AZ56"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AU6" sqref="AU6"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AN8" sqref="AN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61625,7 +61625,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>